<commit_message>
AutoCommit_2 июля 2023 г. 23:14:22_SibNout2020
</commit_message>
<xml_diff>
--- a/2ИСИП-321/2ИСИП-321_Сети.xlsx
+++ b/2ИСИП-321/2ИСИП-321_Сети.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\_2ИСИП-321\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\2ИСИП-321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58E89D2-23DD-49C3-8F5A-29FE5746BB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0C4DA4-7DB9-4BE8-A7C3-569316EC8C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,10 +584,10 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_2 июля 2023 г. 23:17:40_SibNout2020
</commit_message>
<xml_diff>
--- a/2ИСИП-321/2ИСИП-321_Сети.xlsx
+++ b/2ИСИП-321/2ИСИП-321_Сети.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\2ИСИП-321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0C4DA4-7DB9-4BE8-A7C3-569316EC8C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C9F80F-59E3-4B56-8A9D-E1B9B4265954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,10 +584,10 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,9 @@
       <c r="K11" s="4">
         <v>5</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="L11" s="2">
+        <v>5</v>
+      </c>
       <c r="M11" s="4">
         <v>5</v>
       </c>
@@ -1156,7 +1158,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W11" t="s">
         <v>44</v>
@@ -1381,7 +1383,9 @@
       <c r="K15" s="4">
         <v>5</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
       <c r="M15" s="4">
         <v>5</v>
       </c>
@@ -1400,7 +1404,7 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="W15" t="s">
         <v>44</v>
@@ -1512,7 +1516,9 @@
         <v>5</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="O17" s="2">
+        <v>5</v>
+      </c>
       <c r="P17" s="2">
         <v>5</v>
       </c>
@@ -1526,7 +1532,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="X17">
         <v>10</v>

</xml_diff>

<commit_message>
AutoCommit_3 июля 2023 г. 12:57:45_SibNout2020
</commit_message>
<xml_diff>
--- a/2ИСИП-321/2ИСИП-321_Сети.xlsx
+++ b/2ИСИП-321/2ИСИП-321_Сети.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\2ИСИП-321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C9F80F-59E3-4B56-8A9D-E1B9B4265954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DFD367-ABF2-41FE-B573-F76D3BEEED09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,10 +584,10 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -961,12 +961,14 @@
       <c r="Q8" s="2">
         <v>5</v>
       </c>
-      <c r="R8" s="2"/>
+      <c r="R8" s="2">
+        <v>5</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W8" t="s">
         <v>44</v>
@@ -1399,12 +1401,14 @@
       <c r="Q15" s="2">
         <v>5</v>
       </c>
-      <c r="R15" s="2"/>
+      <c r="R15" s="2">
+        <v>5</v>
+      </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W15" t="s">
         <v>44</v>

</xml_diff>